<commit_message>
Test account with address
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/DataExcel.xlsx
+++ b/src/test/resources/testdata/DataExcel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Selenium_New\Luma\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50513A76-F087-4768-BCD1-44BA887C86DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEAA1B1E-1BB0-4263-AEC3-0FDB6FA1A765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Account" sheetId="10" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="76">
   <si>
     <t>TESTCASEID</t>
   </si>
@@ -208,17 +208,59 @@
     <t>account_test12@example.com</t>
   </si>
   <si>
-    <t>edit_account_test4@example.com</t>
-  </si>
-  <si>
     <t>Create Failure with Existed Data</t>
+  </si>
+  <si>
+    <t>URL_EDIT_SUB</t>
+  </si>
+  <si>
+    <t>https://magento-demo.mageplaza.com/newsletter/manage/</t>
+  </si>
+  <si>
+    <t>URL_MANAGE_ADDRESS</t>
+  </si>
+  <si>
+    <t>https://magento-demo.mageplaza.com/customer/address/</t>
+  </si>
+  <si>
+    <t>Company_New</t>
+  </si>
+  <si>
+    <t>(333) 65464648</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>LA</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>Los</t>
+  </si>
+  <si>
+    <t>Paris</t>
+  </si>
+  <si>
+    <t>URL_ADD_ADDRESS</t>
+  </si>
+  <si>
+    <t>https://magento-demo.mageplaza.com/customer/address/new/</t>
+  </si>
+  <si>
+    <t>account_test15@example.com</t>
+  </si>
+  <si>
+    <t>edit_account_test6@example.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -247,6 +289,12 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -576,8 +624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DD47ECD-1623-46A6-843B-A37E936F1C54}">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="J4:L5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -639,7 +687,7 @@
         <v>19</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
@@ -730,7 +778,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>59</v>
@@ -795,10 +843,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{788BB3CB-428E-4559-990F-BFA47C812166}">
-  <dimension ref="A1:U4"/>
+  <dimension ref="A1:X4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -819,10 +867,15 @@
     <col min="15" max="15" width="21.5" customWidth="1"/>
     <col min="16" max="16" width="14.09765625" customWidth="1"/>
     <col min="17" max="17" width="19.59765625" customWidth="1"/>
-    <col min="18" max="18" width="16.69921875" customWidth="1"/>
+    <col min="18" max="18" width="34.3984375" customWidth="1"/>
+    <col min="19" max="19" width="17.19921875" customWidth="1"/>
+    <col min="20" max="20" width="29.09765625" customWidth="1"/>
+    <col min="21" max="21" width="11.796875" customWidth="1"/>
+    <col min="22" max="22" width="19.3984375" customWidth="1"/>
+    <col min="23" max="23" width="19.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -886,8 +939,17 @@
       <c r="U1" s="1" t="s">
         <v>58</v>
       </c>
+      <c r="V1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>72</v>
+      </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
@@ -898,7 +960,7 @@
         <v>44</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>14</v>
@@ -951,25 +1013,75 @@
       <c r="U2" t="s">
         <v>2</v>
       </c>
+      <c r="V2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="W2" t="s">
+        <v>64</v>
+      </c>
+      <c r="X2" t="s">
+        <v>73</v>
+      </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
-      <c r="D3" s="2"/>
+      <c r="D3" s="3"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
+      <c r="H3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q3">
+        <v>600005</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="T3" t="s">
+        <v>57</v>
+      </c>
+      <c r="U3" t="s">
+        <v>2</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="W3" t="s">
+        <v>64</v>
+      </c>
+      <c r="X3" t="s">
+        <v>73</v>
+      </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -987,14 +1099,21 @@
       <c r="Q4" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1" xr:uid="{CB08BF40-683B-45DB-AE1D-8AE25CBE91E9}"/>
     <hyperlink ref="I2" r:id="rId2" xr:uid="{7F6727E2-D707-45F3-9653-D32E4E0A54B9}"/>
     <hyperlink ref="D2" r:id="rId3" xr:uid="{CE1595A5-028B-4E2F-AE99-A13263774713}"/>
     <hyperlink ref="S2" r:id="rId4" xr:uid="{9D0ED43F-672C-4E4A-828B-A1C82F88A370}"/>
     <hyperlink ref="R2" r:id="rId5" xr:uid="{4C31FBDB-0ABA-4F80-A8AB-1F8BD8295D89}"/>
+    <hyperlink ref="V2" r:id="rId6" xr:uid="{2B213EDB-40E0-4299-A7B9-BC2153A1CCD8}"/>
+    <hyperlink ref="H3" r:id="rId7" xr:uid="{B102E139-27AC-4468-8B0E-4604B8AB2214}"/>
+    <hyperlink ref="I3" r:id="rId8" xr:uid="{83FA6AB6-148F-45AF-84A4-F3BBBC298675}"/>
+    <hyperlink ref="S3" r:id="rId9" xr:uid="{212C561D-B66B-40DE-A298-0F11187803C0}"/>
+    <hyperlink ref="R3" r:id="rId10" xr:uid="{574E1428-629C-4A23-8BB2-21DE82FCCB04}"/>
+    <hyperlink ref="V3" r:id="rId11" xr:uid="{D7CD382A-AF30-4826-815D-B2DFCFEBC167}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Test search and sort prods
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/DataExcel.xlsx
+++ b/src/test/resources/testdata/DataExcel.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Selenium_New\Luma\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEAA1B1E-1BB0-4263-AEC3-0FDB6FA1A765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AF9ACA3-70B8-4FEE-8D52-B4500EC7724F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Account" sheetId="10" r:id="rId1"/>
     <sheet name="Edit_Account" sheetId="11" r:id="rId2"/>
+    <sheet name="Search" sheetId="12" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="87">
   <si>
     <t>TESTCASEID</t>
   </si>
@@ -254,6 +255,39 @@
   </si>
   <si>
     <t>edit_account_test6@example.com</t>
+  </si>
+  <si>
+    <t>Search with no search results</t>
+  </si>
+  <si>
+    <t>URL_SEARCH_RESULTS</t>
+  </si>
+  <si>
+    <t>https://magento-demo.mageplaza.com/catalogsearch/result/?q=</t>
+  </si>
+  <si>
+    <t>SEARCH_KEYWORDS</t>
+  </si>
+  <si>
+    <t>Zing Jump Rope</t>
+  </si>
+  <si>
+    <t>Search with muti products</t>
+  </si>
+  <si>
+    <t>Search with muti hints</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>Search with a product</t>
+  </si>
+  <si>
+    <t>sport</t>
+  </si>
+  <si>
+    <t>shir</t>
   </si>
 </sst>
 </file>
@@ -845,7 +879,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{788BB3CB-428E-4559-990F-BFA47C812166}">
   <dimension ref="A1:X4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -1116,4 +1150,104 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId12"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F64EC897-840B-46E8-A465-BC5AA58F3F46}">
+  <dimension ref="A1:D20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.5" customWidth="1"/>
+    <col min="2" max="2" width="32" customWidth="1"/>
+    <col min="3" max="3" width="27.3984375" customWidth="1"/>
+    <col min="4" max="4" width="38.3984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5">
+        <v>4567</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D9" s="3"/>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{5CFF6DC8-D6B4-41B8-A010-CBE13F6D02BE}"/>
+    <hyperlink ref="C3:C5" r:id="rId2" display="https://magento-demo.mageplaza.com/catalogsearch/result/?q=" xr:uid="{1EAD0D69-8D4F-4CE0-A57A-BBC57E8552F6}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+</worksheet>
 </file>
</xml_diff>